<commit_message>
Rebrand the INFORM.xlsx spreadsheet
</commit_message>
<xml_diff>
--- a/docs/extra/INFORM.xlsx
+++ b/docs/extra/INFORM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtcunningham/Documents/1. Current Projects/workshop.wiki/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Code/m3tid/docs/extra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435A3843-0EF7-0C40-9706-A15FD13B03AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E459FCA-719A-9147-94E3-796353237294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="1920" windowWidth="27100" windowHeight="17220" firstSheet="1" activeTab="2" xr2:uid="{A6CEF9E4-12E6-4945-8009-89B93494DE93}"/>
+    <workbookView xWindow="24500" yWindow="3420" windowWidth="22320" windowHeight="21300" xr2:uid="{A6CEF9E4-12E6-4945-8009-89B93494DE93}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="11" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="182">
   <si>
     <t>Measuring Threat-Informed Defense</t>
   </si>
@@ -193,12 +193,6 @@
     <t>[1] https://center-for-threat-informed-defense.github.io/summiting-the-pyramid/levels/</t>
   </si>
   <si>
-    <t>[2] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/top-attack-techniques/</t>
-  </si>
-  <si>
-    <t>[3] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/threat-report-attck-mapper-tram/</t>
-  </si>
-  <si>
     <t>[4] https://github.com/center-for-threat-informed-defense/cti-blueprints/wiki</t>
   </si>
   <si>
@@ -265,12 +259,6 @@
     <t>[3] https://www.first.org/epss/</t>
   </si>
   <si>
-    <t>[4] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/mapping-attck-to-cve-for-impact/</t>
-  </si>
-  <si>
-    <t>[5] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/atomic-data-sources/</t>
-  </si>
-  <si>
     <t>[6] https://center-for-threat-informed-defense.github.io/summiting-the-pyramid/</t>
   </si>
   <si>
@@ -370,12 +358,6 @@
     <t>[2] https://github.com/center-for-threat-informed-defense/adversary_emulation_library</t>
   </si>
   <si>
-    <t>[3] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/attack-flow/</t>
-  </si>
-  <si>
-    <t>[4] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/micro-emulation-plans/</t>
-  </si>
-  <si>
     <t>[5] https://posts.specterops.io/reactive-progress-and-tradecraft-innovation-b616f85b6c0a</t>
   </si>
   <si>
@@ -490,27 +472,6 @@
     <t>Test Results</t>
   </si>
   <si>
-    <t>Respondent</t>
-  </si>
-  <si>
-    <t>David Vasil</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>HCA Healthcare</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Disclosure</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Ephemeral IOCs: hashes, IPs, domains</t>
   </si>
   <si>
@@ -650,6 +611,24 @@
   </si>
   <si>
     <t xml:space="preserve">Test and tune custom detection rules </t>
+  </si>
+  <si>
+    <t>[2] https://ctid.mitre.org/projects/top-attack-techniques/</t>
+  </si>
+  <si>
+    <t>[3] https://ctid.mitre.org/projects/threat-report-attck-mapper-tram/</t>
+  </si>
+  <si>
+    <t>[4] https://ctid.mitre.org/projects/mapping-attck-to-cve-for-impact/</t>
+  </si>
+  <si>
+    <t>[5] https://ctid.mitre.org/projects/atomic-data-sources/</t>
+  </si>
+  <si>
+    <t>[3] https://ctid.mitre.org/projects/attack-flow/</t>
+  </si>
+  <si>
+    <t>[4] https://ctid.mitre.org/projects/micro-emulation-plans/</t>
   </si>
 </sst>
 </file>
@@ -659,7 +638,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -817,15 +796,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="13">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -882,23 +854,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFD966"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1178,24 +1139,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1288,14 +1238,6 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="23" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="11" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1317,7 +1259,7 @@
     <xf numFmtId="49" fontId="11" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1440,9 +1382,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
-    <cellStyle name="Accent5" xfId="4" builtinId="45"/>
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
@@ -9517,50 +9457,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>659130</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACFEA6E5-89B3-5679-C46A-C2E44563E190}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="47625" y="219075"/>
-          <a:ext cx="1952625" cy="1047750"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -9985,26 +9881,67 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>58458</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Picture 3">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB9177B1-0CEA-F052-88BD-BBC62F9C6AD2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{036E261B-78FF-C3AE-4AD2-3A09571CCC52}"/>
             </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DA7F7775-1674-55A8-8195-DEC4F61D1BE7}"/>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="381000"/>
+          <a:ext cx="2578100" cy="287058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>522528</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95673DFF-9519-C21F-A05E-01649B9CCE37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10020,8 +9957,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2238375" y="9486900"/>
-          <a:ext cx="3486150" cy="2009775"/>
+          <a:off x="2451100" y="9512300"/>
+          <a:ext cx="2783128" cy="2565400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11483,10 +11420,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="B3:N12"/>
+  <dimension ref="B5:B9"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11495,48 +11432,18 @@
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="D3" s="7" t="s">
+    <row r="5" spans="2:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="D4" s="7" t="s">
+    <row r="6" spans="2:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="M9" s="54" t="s">
-        <v>137</v>
-      </c>
-      <c r="N9" s="55" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M10" s="54" t="s">
-        <v>135</v>
-      </c>
-      <c r="N10" s="55" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M11" s="54" t="s">
-        <v>139</v>
-      </c>
-      <c r="N11" s="56">
-        <v>45615</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="22" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="M12" s="57" t="s">
-        <v>140</v>
-      </c>
-      <c r="N12" t="s">
-        <v>141</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11562,7 +11469,7 @@
     </row>
     <row r="7" spans="2:4" ht="21" x14ac:dyDescent="0.25">
       <c r="D7" s="7" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
@@ -11581,8 +11488,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="71" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="71" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11622,42 +11529,42 @@
     <row r="6" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
       <c r="B6" s="42"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
     </row>
     <row r="7" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
       <c r="B7" s="38"/>
-      <c r="C7" s="80" t="s">
+      <c r="C7" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="81"/>
-      <c r="E7" s="80" t="s">
+      <c r="D7" s="77"/>
+      <c r="E7" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="81"/>
-      <c r="G7" s="80" t="s">
+      <c r="F7" s="77"/>
+      <c r="G7" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="81"/>
-      <c r="I7" s="80" t="s">
+      <c r="H7" s="77"/>
+      <c r="I7" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="81"/>
-      <c r="K7" s="80" t="s">
+      <c r="J7" s="77"/>
+      <c r="K7" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="81"/>
+      <c r="L7" s="77"/>
     </row>
     <row r="8" spans="1:12" s="37" customFormat="1" ht="88" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
@@ -11696,185 +11603,185 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="59">
+      <c r="B9" s="55">
         <v>0</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="61"/>
-      <c r="E9" s="60" t="s">
+      <c r="D9" s="57"/>
+      <c r="E9" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="61"/>
-      <c r="G9" s="60" t="s">
+      <c r="F9" s="57"/>
+      <c r="G9" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="61"/>
-      <c r="I9" s="60" t="s">
+      <c r="H9" s="57"/>
+      <c r="I9" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="61"/>
-      <c r="K9" s="62" t="s">
+      <c r="J9" s="57"/>
+      <c r="K9" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="61"/>
+      <c r="L9" s="57"/>
     </row>
     <row r="10" spans="1:12" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="58">
+      <c r="B10" s="54">
         <v>1</v>
       </c>
-      <c r="C10" s="63" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" s="64"/>
-      <c r="E10" s="63" t="s">
-        <v>150</v>
-      </c>
-      <c r="F10" s="64"/>
-      <c r="G10" s="63" t="s">
+      <c r="C10" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="60"/>
+      <c r="E10" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="60"/>
+      <c r="G10" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="64"/>
-      <c r="I10" s="63" t="s">
-        <v>146</v>
-      </c>
-      <c r="J10" s="65"/>
-      <c r="K10" s="66" t="s">
+      <c r="H10" s="60"/>
+      <c r="I10" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="J10" s="61"/>
+      <c r="K10" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="64"/>
+      <c r="L10" s="60"/>
     </row>
     <row r="11" spans="1:12" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="58">
+      <c r="B11" s="54">
         <v>1</v>
       </c>
-      <c r="C11" s="63" t="s">
-        <v>143</v>
-      </c>
-      <c r="D11" s="64"/>
-      <c r="E11" s="63" t="s">
-        <v>151</v>
-      </c>
-      <c r="F11" s="64"/>
-      <c r="G11" s="67" t="s">
-        <v>153</v>
-      </c>
-      <c r="H11" s="65"/>
-      <c r="I11" s="63" t="s">
+      <c r="C11" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="60"/>
+      <c r="E11" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" s="60"/>
+      <c r="G11" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" s="61"/>
+      <c r="I11" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="65"/>
-      <c r="K11" s="66" t="s">
+      <c r="J11" s="61"/>
+      <c r="K11" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="64"/>
+      <c r="L11" s="60"/>
     </row>
     <row r="12" spans="1:12" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="58">
+      <c r="B12" s="54">
         <v>2</v>
       </c>
-      <c r="C12" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="63" t="s">
-        <v>158</v>
-      </c>
-      <c r="F12" s="64"/>
-      <c r="G12" s="75" t="s">
-        <v>154</v>
-      </c>
-      <c r="H12" s="65"/>
-      <c r="I12" s="63" t="s">
-        <v>147</v>
-      </c>
-      <c r="J12" s="65"/>
-      <c r="K12" s="66" t="s">
-        <v>156</v>
-      </c>
-      <c r="L12" s="64"/>
+      <c r="C12" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="60"/>
+      <c r="E12" s="59" t="s">
+        <v>145</v>
+      </c>
+      <c r="F12" s="60"/>
+      <c r="G12" s="71" t="s">
+        <v>141</v>
+      </c>
+      <c r="H12" s="61"/>
+      <c r="I12" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="J12" s="61"/>
+      <c r="K12" s="62" t="s">
+        <v>143</v>
+      </c>
+      <c r="L12" s="60"/>
     </row>
     <row r="13" spans="1:12" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="68">
+      <c r="B13" s="64">
         <v>2</v>
       </c>
-      <c r="C13" s="69" t="s">
-        <v>145</v>
-      </c>
-      <c r="D13" s="70"/>
-      <c r="E13" s="63" t="s">
-        <v>152</v>
-      </c>
-      <c r="F13" s="70"/>
-      <c r="G13" s="69" t="s">
+      <c r="C13" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="66"/>
+      <c r="E13" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="65"/>
-      <c r="I13" s="69" t="s">
-        <v>155</v>
-      </c>
-      <c r="J13" s="65"/>
-      <c r="K13" s="71" t="s">
-        <v>157</v>
-      </c>
-      <c r="L13" s="64"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="J13" s="61"/>
+      <c r="K13" s="67" t="s">
+        <v>144</v>
+      </c>
+      <c r="L13" s="60"/>
     </row>
     <row r="14" spans="1:12" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="72" t="s">
+      <c r="A14" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="73">
+      <c r="B14" s="69">
         <f>AVERAGE(D14,F14,H14,J14,L14)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="74">
+      <c r="D14" s="70">
         <f>SUMIF(D9:D13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="63" t="s">
+      <c r="E14" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="63">
+      <c r="F14" s="59">
         <f>SUMIF(F9:F13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="63" t="s">
+      <c r="G14" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="63">
+      <c r="H14" s="59">
         <f>SUMIF(H9:H13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="63" t="s">
+      <c r="I14" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="63">
+      <c r="J14" s="59">
         <f>SUMIF(J9:J13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
-      <c r="K14" s="66" t="s">
+      <c r="K14" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="63">
+      <c r="L14" s="59">
         <f>SUMIF(L9:L13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
@@ -11894,44 +11801,44 @@
       <c r="L15" s="5"/>
     </row>
     <row r="17" spans="3:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="77" t="s">
+      <c r="C18" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="77"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="77" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="77"/>
+      <c r="C19" s="73" t="s">
+        <v>176</v>
+      </c>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="77" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="77"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="77"/>
+      <c r="C20" s="73" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="77" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
+      <c r="C21" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -11961,8 +11868,8 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C21" r:id="rId1" xr:uid="{3D69BB28-107D-4325-9460-77D240B55F11}"/>
-    <hyperlink ref="C20" r:id="rId2" xr:uid="{2E192557-D1CC-4D93-A5DC-FF959F5553A1}"/>
-    <hyperlink ref="C19" r:id="rId3" xr:uid="{A4EAF72E-A70C-41D6-B7EF-8D9CB9B65D38}"/>
+    <hyperlink ref="C20" r:id="rId2" display="[3] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/threat-report-attck-mapper-tram/" xr:uid="{2E192557-D1CC-4D93-A5DC-FF959F5553A1}"/>
+    <hyperlink ref="C19" r:id="rId3" display="[2] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/top-attack-techniques/" xr:uid="{A4EAF72E-A70C-41D6-B7EF-8D9CB9B65D38}"/>
     <hyperlink ref="C18" r:id="rId4" xr:uid="{E3EA1249-47A4-490F-BF52-4B17536085F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11978,7 +11885,7 @@
   <dimension ref="A2:L25"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C23" sqref="C23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12004,86 +11911,86 @@
     </row>
     <row r="3" spans="1:12" ht="26" x14ac:dyDescent="0.3">
       <c r="C3" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:12" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="C4" s="32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
       <c r="B6" s="29"/>
-      <c r="C6" s="82" t="s">
+      <c r="C6" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
     </row>
     <row r="7" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
       <c r="B7" s="29"/>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="80"/>
+      <c r="E7" s="79" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="80"/>
+      <c r="G7" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="84"/>
-      <c r="E7" s="83" t="s">
+      <c r="H7" s="80"/>
+      <c r="I7" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="84"/>
-      <c r="G7" s="83" t="s">
+      <c r="J7" s="80"/>
+      <c r="K7" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="84"/>
-      <c r="I7" s="83" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="84"/>
-      <c r="K7" s="83" t="s">
-        <v>45</v>
-      </c>
-      <c r="L7" s="84"/>
+      <c r="L7" s="80"/>
     </row>
     <row r="8" spans="1:12" ht="110" x14ac:dyDescent="0.25">
       <c r="A8" s="29"/>
       <c r="B8" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="46" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="47" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F8" s="46" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="47" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H8" s="46" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="47" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J8" s="46" t="s">
         <v>12</v>
       </c>
       <c r="K8" s="47" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L8" s="46" t="s">
         <v>12</v>
@@ -12125,23 +12032,23 @@
         <v>1</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="18" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="F10" s="26"/>
       <c r="G10" s="18" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="18" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="J10" s="26"/>
       <c r="K10" s="19" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="L10" s="26"/>
     </row>
@@ -12153,23 +12060,23 @@
         <v>1</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="18" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="F11" s="26"/>
       <c r="G11" s="18" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="18" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="J11" s="26"/>
       <c r="K11" s="19" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="L11" s="26"/>
     </row>
@@ -12181,23 +12088,23 @@
         <v>2</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="18" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="18" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="18" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J12" s="26"/>
       <c r="K12" s="19" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="L12" s="26"/>
     </row>
@@ -12209,64 +12116,64 @@
         <v>2</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="18" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="18" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="18" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="J13" s="26"/>
       <c r="K13" s="19" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="L13" s="26"/>
     </row>
     <row r="14" spans="1:12" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14" s="24">
         <f>AVERAGE(D14,F14,H14,J14,L14)</f>
         <v>0</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" s="18">
         <f>SUMIF(D9:D13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F14" s="18">
         <f>SUMIF(F9:F13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H14" s="18">
         <f>SUMIF(H9:H13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J14" s="18">
         <f>SUMIF(J9:J13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L14" s="18">
         <f>SUMIF(L9:L13,"yes",$B$9:$B$13)</f>
@@ -12274,76 +12181,76 @@
       </c>
     </row>
     <row r="17" spans="3:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
     </row>
     <row r="18" spans="3:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="77" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="77"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
+      <c r="C18" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="77" t="s">
-        <v>148</v>
-      </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="77"/>
+      <c r="C19" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="77"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="77"/>
+      <c r="C20" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
+      <c r="C21" s="73" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C22" s="77" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
+      <c r="C22" s="73" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C23" s="77" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
+      <c r="C23" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C24" s="77" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
+      <c r="C24" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C25" s="77" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
+      <c r="C25" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -12375,8 +12282,8 @@
     <hyperlink ref="C18" r:id="rId1" xr:uid="{9A9EBAF9-4CF8-48F1-9897-FF88B620BCC9}"/>
     <hyperlink ref="C19" r:id="rId2" display="[2] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/nist-800-53-control-mappings/" xr:uid="{BC02007E-E9E5-4589-BE76-4AAA80D987A9}"/>
     <hyperlink ref="C20" r:id="rId3" xr:uid="{FA3D2F92-F664-4613-81DD-729CFE590BCA}"/>
-    <hyperlink ref="C21" r:id="rId4" xr:uid="{71A85C83-08E6-4851-8750-329D38D29058}"/>
-    <hyperlink ref="C22" r:id="rId5" xr:uid="{CF818E72-59E9-4E8C-98A4-979902DAAB69}"/>
+    <hyperlink ref="C21" r:id="rId4" display="[4] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/mapping-attck-to-cve-for-impact/" xr:uid="{71A85C83-08E6-4851-8750-329D38D29058}"/>
+    <hyperlink ref="C22" r:id="rId5" display="[5] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/atomic-data-sources/" xr:uid="{CF818E72-59E9-4E8C-98A4-979902DAAB69}"/>
     <hyperlink ref="C23" r:id="rId6" xr:uid="{357017CF-5A9D-4D91-A993-C72C85980C74}"/>
     <hyperlink ref="C24" r:id="rId7" xr:uid="{95B96929-4FD6-4EE0-9CE1-FC332B439501}"/>
     <hyperlink ref="C25" r:id="rId8" xr:uid="{132BF764-517B-4307-9F09-B332EA9B4E26}"/>
@@ -12394,7 +12301,7 @@
   <dimension ref="A3:L22"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12415,86 +12322,86 @@
   <sheetData>
     <row r="3" spans="1:12" ht="26" x14ac:dyDescent="0.3">
       <c r="C3" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:12" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="C4" s="32" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="38"/>
       <c r="B6" s="51"/>
-      <c r="C6" s="85" t="s">
+      <c r="C6" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
-      <c r="L6" s="87"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="83"/>
     </row>
     <row r="7" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="38"/>
       <c r="B7" s="51"/>
-      <c r="C7" s="88" t="s">
+      <c r="C7" s="84" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="85"/>
+      <c r="G7" s="86" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="85"/>
+      <c r="I7" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" s="85"/>
+      <c r="K7" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="89"/>
-      <c r="E7" s="90" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="89"/>
-      <c r="G7" s="90" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="89"/>
-      <c r="I7" s="90" t="s">
-        <v>70</v>
-      </c>
-      <c r="J7" s="89"/>
-      <c r="K7" s="90" t="s">
-        <v>71</v>
-      </c>
-      <c r="L7" s="91"/>
+      <c r="L7" s="87"/>
     </row>
     <row r="8" spans="1:12" ht="66" x14ac:dyDescent="0.25">
       <c r="A8" s="38"/>
       <c r="B8" s="38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D8" s="53" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F8" s="53" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H8" s="53" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="52" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J8" s="53" t="s">
         <v>12</v>
       </c>
       <c r="K8" s="52" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L8" s="53" t="s">
         <v>12</v>
@@ -12536,23 +12443,23 @@
         <v>1</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F10" s="26"/>
       <c r="G10" s="18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="18" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="J10" s="26"/>
       <c r="K10" s="19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L10" s="26"/>
     </row>
@@ -12564,23 +12471,23 @@
         <v>1</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F11" s="26"/>
       <c r="G11" s="18" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="18" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="J11" s="26"/>
       <c r="K11" s="19" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="L11" s="26"/>
     </row>
@@ -12592,23 +12499,23 @@
         <v>2</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="18" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="J12" s="26"/>
       <c r="K12" s="19" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L12" s="26"/>
     </row>
@@ -12620,64 +12527,64 @@
         <v>2</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="18" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="J13" s="26"/>
       <c r="K13" s="19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="L13" s="26"/>
     </row>
     <row r="14" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B14" s="23">
         <f>AVERAGE(D14,F14,H14,J14,L14)</f>
         <v>0</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D14" s="18">
         <f>SUMIF(D9:D13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F14" s="18">
         <f>SUMIF(F9:F13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H14" s="18">
         <f>SUMIF(H9:H13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J14" s="18">
         <f>SUMIF(J9:J13,"yes",$B$9:$B$13)</f>
         <v>0</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="L14" s="18">
         <f>SUMIF(L9:L13,"yes",$B$9:$B$13)</f>
@@ -12685,52 +12592,52 @@
       </c>
     </row>
     <row r="17" spans="3:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
     </row>
     <row r="18" spans="3:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="77" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="77"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
+      <c r="C18" s="73" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="92" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
+      <c r="C19" s="88" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="77" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="77"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="77"/>
+      <c r="C20" s="73" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="77" t="s">
-        <v>96</v>
-      </c>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
+      <c r="C21" s="73" t="s">
+        <v>181</v>
+      </c>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C22" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
+      <c r="C22" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -12758,8 +12665,8 @@
   <hyperlinks>
     <hyperlink ref="C18" r:id="rId1" xr:uid="{D61793AA-EA6D-4627-A061-5E21BD0605D9}"/>
     <hyperlink ref="C19" r:id="rId2" xr:uid="{169E7A20-0090-4D6C-BF7A-02EC33F5D95C}"/>
-    <hyperlink ref="C20" r:id="rId3" xr:uid="{7F25465C-B2F1-4F54-AEEB-8F8307A1E761}"/>
-    <hyperlink ref="C21" r:id="rId4" xr:uid="{61A7C054-16FA-43FF-9709-3415A6CB7EF4}"/>
+    <hyperlink ref="C20" r:id="rId3" display="[3] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/attack-flow/" xr:uid="{7F25465C-B2F1-4F54-AEEB-8F8307A1E761}"/>
+    <hyperlink ref="C21" r:id="rId4" display="[4] https://mitre-engenuity.org/cybersecurity/center-for-threat-informed-defense/our-work/micro-emulation-plans/" xr:uid="{61A7C054-16FA-43FF-9709-3415A6CB7EF4}"/>
     <hyperlink ref="C22" r:id="rId5" xr:uid="{B3D42F13-E969-48CE-A25E-03744EDAC918}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12775,7 +12682,7 @@
   <dimension ref="B1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12790,12 +12697,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
@@ -12805,39 +12712,39 @@
     </row>
     <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G4" s="7"/>
     </row>
     <row r="8" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H8" s="33"/>
     </row>
     <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B9" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="103"/>
-      <c r="D9" s="104"/>
-      <c r="E9" s="104"/>
-      <c r="F9" s="105"/>
+        <v>99</v>
+      </c>
+      <c r="C9" s="99"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="101"/>
       <c r="G9" s="50">
         <f>((0.5*G16)+(0.3*G10)+(0.2*G22))/((0.5*6)+(0.3*6)+(0.2*6))</f>
         <v>0</v>
@@ -12846,12 +12753,12 @@
     </row>
     <row r="10" spans="2:8" ht="19" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" s="100"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="102"/>
+        <v>100</v>
+      </c>
+      <c r="C10" s="96"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="98"/>
       <c r="G10" s="15">
         <f>AVERAGE(G11:G15)</f>
         <v>0</v>
@@ -12985,12 +12892,12 @@
     </row>
     <row r="16" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="97"/>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="99"/>
+        <v>101</v>
+      </c>
+      <c r="C16" s="93"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="95"/>
       <c r="G16" s="17">
         <f>AVERAGE(G17:G21)</f>
         <v>0</v>
@@ -12999,7 +12906,7 @@
     </row>
     <row r="17" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C17" s="9" t="str">
         <f>IF('DM Definition &amp; Scoring'!D10="yes","x","")</f>
@@ -13024,7 +12931,7 @@
     </row>
     <row r="18" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" s="9" t="str">
         <f>IF('DM Definition &amp; Scoring'!F10="yes","x","")</f>
@@ -13049,7 +12956,7 @@
     </row>
     <row r="19" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19" s="9" t="str">
         <f>IF('DM Definition &amp; Scoring'!H10="yes","x","")</f>
@@ -13074,7 +12981,7 @@
     </row>
     <row r="20" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20" s="9" t="str">
         <f>IF('DM Definition &amp; Scoring'!J10="yes","x","")</f>
@@ -13099,7 +13006,7 @@
     </row>
     <row r="21" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C21" s="9" t="str">
         <f>IF('DM Definition &amp; Scoring'!L10="yes","x","")</f>
@@ -13124,12 +13031,12 @@
     </row>
     <row r="22" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="94"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="95"/>
-      <c r="F22" s="96"/>
+        <v>104</v>
+      </c>
+      <c r="C22" s="90"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="92"/>
       <c r="G22" s="16">
         <f>AVERAGE(G23:G27)</f>
         <v>0</v>
@@ -13138,7 +13045,7 @@
     </row>
     <row r="23" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C23" s="9" t="str">
         <f>IF('T&amp;E Definition &amp; Scoring'!D10="yes","x","")</f>
@@ -13163,7 +13070,7 @@
     </row>
     <row r="24" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C24" s="9" t="str">
         <f>IF('T&amp;E Definition &amp; Scoring'!F10="yes","x","")</f>
@@ -13188,7 +13095,7 @@
     </row>
     <row r="25" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C25" s="9" t="str">
         <f>IF('T&amp;E Definition &amp; Scoring'!H10="yes","x","")</f>
@@ -13213,7 +13120,7 @@
     </row>
     <row r="26" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C26" s="9" t="str">
         <f>IF('T&amp;E Definition &amp; Scoring'!J10="yes","x","")</f>
@@ -13238,7 +13145,7 @@
     </row>
     <row r="27" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C27" s="9" t="str">
         <f>IF('T&amp;E Definition &amp; Scoring'!L10="yes","x","")</f>
@@ -13263,18 +13170,18 @@
     </row>
     <row r="29" spans="2:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="G29" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="G30" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H30" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="I30" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13515,25 +13422,25 @@
   <sheetData>
     <row r="1" spans="1:32" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B1" s="14">
         <f>(B8*((0.66*B2)+(0.34*B14)))/(10*((0.66*10)+(0.34*10)))</f>
         <v>1.264E-2</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B2" s="15">
         <f>AVERAGE(B3:B7)</f>
@@ -13557,7 +13464,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B3" s="9">
         <f>G3</f>
@@ -13587,7 +13494,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B4" s="9">
         <f>G4</f>
@@ -13617,7 +13524,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B5" s="9">
         <f>G5</f>
@@ -13644,7 +13551,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B6" s="9">
         <f>G6</f>
@@ -13671,7 +13578,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B7" s="9">
         <f>G7</f>
@@ -13701,23 +13608,23 @@
     </row>
     <row r="8" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B8" s="17">
         <f>AVERAGE(B9:B13)</f>
         <v>1</v>
       </c>
-      <c r="C8" s="106"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B9" s="9">
         <f>G9</f>
@@ -13747,7 +13654,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B10" s="9">
         <f>G10</f>
@@ -13777,7 +13684,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B11" s="9">
         <f>G11</f>
@@ -13807,7 +13714,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B12" s="9">
         <f>G12</f>
@@ -13837,7 +13744,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B13" s="9">
         <f>G13</f>
@@ -13855,23 +13762,23 @@
     </row>
     <row r="14" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B14" s="16">
         <f>AVERAGE(B15:B19)</f>
         <v>1</v>
       </c>
-      <c r="C14" s="106"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B15" s="9">
         <f>G15</f>
@@ -13900,21 +13807,21 @@
       </c>
       <c r="AB15" s="9"/>
       <c r="AC15" s="9" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="AD15" s="9" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="AE15" s="9" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="AF15" s="9" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B16" s="9">
         <f>G16</f>
@@ -13933,7 +13840,7 @@
         <v>4</v>
       </c>
       <c r="AB16" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="AC16" s="9">
         <f>$AF$16*AVERAGE(G3:G7)</f>
@@ -13953,7 +13860,7 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B17" s="9">
         <f>G17</f>
@@ -13975,7 +13882,7 @@
         <v>4</v>
       </c>
       <c r="AB17" s="10" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="AC17" s="9">
         <f>$AF$17*AVERAGE(G9:G13)</f>
@@ -13995,7 +13902,7 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B18" s="9">
         <f>G18</f>
@@ -14014,7 +13921,7 @@
         <v>4</v>
       </c>
       <c r="AB18" s="10" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="AC18" s="9">
         <f>$AF$18*AVERAGE(G15:G19)</f>
@@ -14034,7 +13941,7 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B19" s="9">
         <f>G19</f>
@@ -14058,18 +13965,18 @@
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -14091,7 +13998,7 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -14113,7 +14020,7 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>

</xml_diff>